<commit_message>
added fig3-6 (merged table3-3 to figure)
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/j_igarashi/Documents/git/JinIgarashi/cacus-narok-figures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D93DFAFD-EA1D-0942-BB3D-8D7E4CB86AC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3861A620-296C-D342-8B56-3E969BF2C388}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30040" yWindow="-1100" windowWidth="29640" windowHeight="19680" activeTab="4" xr2:uid="{4C00E243-9F2A-B441-AADD-7B36CF36FAEE}"/>
+    <workbookView xWindow="-29960" yWindow="-13080" windowWidth="29640" windowHeight="19680" activeTab="7" xr2:uid="{4C00E243-9F2A-B441-AADD-7B36CF36FAEE}"/>
   </bookViews>
   <sheets>
     <sheet name="E&amp;T_detail" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,11 @@
     <sheet name="treatment_detail" sheetId="3" r:id="rId3"/>
     <sheet name="treatment_total" sheetId="4" r:id="rId4"/>
     <sheet name="fsm containment" sheetId="5" r:id="rId5"/>
+    <sheet name="fsm_E&amp;T" sheetId="6" r:id="rId6"/>
+    <sheet name="fsm_E&amp;T_directcapex" sheetId="9" r:id="rId7"/>
+    <sheet name="fsm_E&amp;T_indirectcapex" sheetId="10" r:id="rId8"/>
+    <sheet name="fsm_E&amp;T_directopex" sheetId="7" r:id="rId9"/>
+    <sheet name="fsm_E&amp;T_indirectopex" sheetId="8" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="78">
   <si>
     <t>Direct CapEx</t>
   </si>
@@ -235,6 +240,45 @@
   </si>
   <si>
     <t>Total Household</t>
+  </si>
+  <si>
+    <t>NARWASSCO</t>
+  </si>
+  <si>
+    <t>Wambugu</t>
+  </si>
+  <si>
+    <t>Direct CAPEX</t>
+  </si>
+  <si>
+    <t>Indirect CAPEX</t>
+  </si>
+  <si>
+    <t>Direct OPEX</t>
+  </si>
+  <si>
+    <t>Indirect OPEX</t>
+  </si>
+  <si>
+    <t>Variable staff payments</t>
+  </si>
+  <si>
+    <t>Fixed non-salary staff expenses</t>
+  </si>
+  <si>
+    <t>Equipment, land and buildings</t>
+  </si>
+  <si>
+    <t>Administrative charges and permits</t>
+  </si>
+  <si>
+    <t>Other expenses for indirect staff</t>
+  </si>
+  <si>
+    <t>Major and Extraordinary Repairs</t>
+  </si>
+  <si>
+    <t>Taxes and Financing for Physical Assets</t>
   </si>
 </sst>
 </file>
@@ -801,6 +845,103 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68688125-B742-7846-B9D9-B102C68A74C0}">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="30.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="1">
+        <v>81866</v>
+      </c>
+      <c r="C2" s="1">
+        <v>35000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B3" s="1">
+        <v>3874</v>
+      </c>
+      <c r="C3" s="1">
+        <v>9600</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B4" s="1">
+        <v>4500</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="1">
+        <v>111977</v>
+      </c>
+      <c r="C5" s="1">
+        <v>119440</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="1">
+        <v>45915</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B7" s="1">
+        <v>12000</v>
+      </c>
+      <c r="C7" s="1">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E3270ED-9D2B-C149-9440-B974E962299F}">
   <dimension ref="A1:B5"/>
@@ -1133,7 +1274,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22D7971D-7BA3-254D-A890-FC8B87258F5F}">
   <dimension ref="A1:Q26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
@@ -2482,4 +2623,360 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76747498-9AA2-BB40-81F0-37A72C4EC8FD}">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B2">
+        <v>108496.59480000001</v>
+      </c>
+      <c r="C2">
+        <v>13966.145</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B3">
+        <v>4000.5176259999998</v>
+      </c>
+      <c r="C3">
+        <v>6654.5423899999996</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B4">
+        <v>76787.253859999997</v>
+      </c>
+      <c r="C4">
+        <v>59820.825700000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B5">
+        <v>5711.446833</v>
+      </c>
+      <c r="C5">
+        <v>4052.0443799999998</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA5306C6-E880-0A40-8FEA-B560E7727494}">
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="30.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1">
+        <v>68455.253955719687</v>
+      </c>
+      <c r="C2" s="1">
+        <v>10731.253285784474</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1">
+        <v>1804.0579588966814</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B4" s="1">
+        <v>40041.34080620754</v>
+      </c>
+      <c r="C4" s="1">
+        <v>1430.8337714379297</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{773E4B96-2D59-C449-84BE-EA6FA64329F5}">
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="30.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1">
+        <v>2187.736754471212</v>
+      </c>
+      <c r="C2" s="1">
+        <v>6654.5423919128834</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B3" s="1">
+        <v>18.59509136818</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1626.0741665651108</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="1">
+        <v>168.11161356659039</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32C32193-87CB-724B-9EB0-B760DB9749A7}">
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="30.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="1">
+        <v>673144</v>
+      </c>
+      <c r="C2" s="1">
+        <v>592000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B3" s="1">
+        <v>360000</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0</v>
+      </c>
+      <c r="C4" s="1">
+        <v>28800</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B5" s="1">
+        <v>36200</v>
+      </c>
+      <c r="C5" s="1">
+        <v>80400</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="1">
+        <v>747652</v>
+      </c>
+      <c r="C6" s="1">
+        <v>1793700</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="1">
+        <v>1403010</v>
+      </c>
+      <c r="C7" s="1">
+        <v>90000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B8" s="1">
+        <v>116000</v>
+      </c>
+      <c r="C8" s="1">
+        <v>6000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>